<commit_message>
support for lambda expressions
</commit_message>
<xml_diff>
--- a/docs/benchmarks.xlsx
+++ b/docs/benchmarks.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\objec\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\objeck-lang\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97716121-B5CF-4B14-A5F1-353F95FE57BB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22140" windowHeight="9852" activeTab="2"/>
+    <workbookView xWindow="2604" yWindow="1884" windowWidth="21408" windowHeight="12888" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="spectral-norm" sheetId="1" r:id="rId1"/>
@@ -21,7 +22,15 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">mandelbrot!$E$1:$E$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'spectral-norm'!$B$1:$B$8</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -61,7 +70,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]&quot;-&quot;[$$-409]#,##0.00"/>
   </numFmts>
@@ -127,11 +136,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Heading" xfId="1"/>
-    <cellStyle name="Heading1" xfId="2"/>
+    <cellStyle name="Heading" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Heading1" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Result" xfId="3"/>
-    <cellStyle name="Result2" xfId="4"/>
+    <cellStyle name="Result" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Result2" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
   </cellStyles>
   <dxfs count="3">
     <dxf>
@@ -3139,16 +3148,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>754380</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>167640</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3180,16 +3189,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>662940</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3221,16 +3230,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>350520</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>53340</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>662940</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3259,12 +3268,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="__Anonymous_Sheet_DB__0" displayName="__Anonymous_Sheet_DB__0" ref="E1:E8" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
-  <sortState ref="E2:E8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="__Anonymous_Sheet_DB__0" displayName="__Anonymous_Sheet_DB__0" ref="E1:E8" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E2:E8">
     <sortCondition ref="E3:E8"/>
   </sortState>
   <tableColumns count="1">
-    <tableColumn id="1" name="Time (secs)" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Time (secs)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3566,11 +3575,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -3738,11 +3747,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -3899,8 +3908,8 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="E1:E7">
-    <sortState ref="A2:E8">
+  <autoFilter ref="E1:E7" xr:uid="{00000000-0009-0000-0000-000001000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E8">
       <sortCondition ref="E1:E7"/>
     </sortState>
   </autoFilter>
@@ -3911,11 +3920,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -4073,8 +4082,8 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="E1:E8">
-    <sortState ref="A2:E8">
+  <autoFilter ref="E1:E8" xr:uid="{00000000-0009-0000-0000-000002000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E8">
       <sortCondition ref="E1:E8"/>
     </sortState>
   </autoFilter>

</xml_diff>